<commit_message>
OS based Chrome driver detection for screenshots
</commit_message>
<xml_diff>
--- a/websites.xlsx
+++ b/websites.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AED3005-FE35-4B24-82BB-5ADF23A587F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="5_{637BF6EF-148F-422D-9B91-E8C74E3003BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{522CEEF1-B84F-4EAC-89BE-CAA55F40A8D2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <t>input_urls</t>
   </si>
   <si>
-    <t>http://shodan.io</t>
+    <t>https://duckduckgo.com</t>
   </si>
   <si>
     <t>http://fakewebsite1289371231273812937127931273817293.com</t>
@@ -39,10 +39,10 @@
     <t>http://github.com</t>
   </si>
   <si>
-    <t>http://example.com/</t>
-  </si>
-  <si>
-    <t>https://duckduckgo.com</t>
+    <t xml:space="preserve">http://shodan.io </t>
+  </si>
+  <si>
+    <t>sub.example.com</t>
   </si>
 </sst>
 </file>
@@ -374,71 +374,70 @@
   <dimension ref="A1:A180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" s="1"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" s="1"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" s="1"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CD9B2AA4-E3EF-4A57-BA3B-75A6A53ECBF7}"/>
-    <hyperlink ref="A3" r:id="rId2" display="http://shodan.io/" xr:uid="{04F0ADC9-F19F-4794-BDCD-C51B95DFDB6A}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{1F03F32F-FBD4-4F77-B2C0-6A8A40573646}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{27B7F57F-4747-4BA8-B55B-1DF329D6BE76}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{BF6386A8-DB92-4A98-B02E-16F23022253E}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{25607D2D-1EF0-4028-A389-90E8EF26636C}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{4B7982B7-9576-4EC0-AA52-EF5DF1B82E17}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{76638385-870C-46D0-9CFF-CFA1D38D7E1A}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{F76F7E18-820A-495B-9B48-2E4112FE99CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>